<commit_message>
feat: pequenos ajustes - ECO-097
</commit_message>
<xml_diff>
--- a/public/file/Servico/MonAtpFauna/Registro.xlsx
+++ b/public/file/Servico/MonAtpFauna/Registro.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="122">
   <si>
     <t>fk_grupo_amostrado</t>
   </si>
@@ -781,7 +781,7 @@
   <dimension ref="A1:AF15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +789,7 @@
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
     <col min="8" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -1972,6 +1972,9 @@
       <c r="K14" s="5" t="s">
         <v>121</v>
       </c>
+      <c r="L14" t="s">
+        <v>51</v>
+      </c>
       <c r="AC14" s="3">
         <v>45574.699305555558</v>
       </c>
@@ -2010,8 +2013,8 @@
       <c r="K15" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L15">
-        <v>2</v>
+      <c r="L15" t="s">
+        <v>63</v>
       </c>
       <c r="M15">
         <v>123</v>

</xml_diff>